<commit_message>
Support parallelizable csv generation. Unescape HTML from shared strings
</commit_message>
<xml_diff>
--- a/spec/data/Spec.xlsx
+++ b/spec/data/Spec.xlsx
@@ -5,25 +5,27 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="3" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="257" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="4" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="257" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="test_otros" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="test_spec" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="test_param" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Lenguajes" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="ont_demo" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">test_param!$A$1:$L$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="Excel_BuiltIn__FilterDatabase" vbProcedure="false">test_spec!$A$1:$L$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">test_param!$A$1:$L$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_1" vbProcedure="false">test_param!$A$1:$L$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
   <si>
     <t>LevenshteinDistance</t>
   </si>
@@ -167,19 +169,42 @@
   </si>
   <si>
     <t>default</t>
+  </si>
+  <si>
+    <t>ClienteTexto_Campos</t>
+  </si>
+  <si>
+    <t>ClienteTexto_Especificacion</t>
+  </si>
+  <si>
+    <t>Discriminación &gt; Sexual | Insulto</t>
+  </si>
+  <si>
+    <t>puto</t>
+  </si>
+  <si>
+    <t>TST_RechAuto_Insulto_SE_Normal</t>
+  </si>
+  <si>
+    <t>Insulto</t>
+  </si>
+  <si>
+    <t>boludo</t>
+  </si>
+  <si>
+    <t>TST_ModMan_Insulto_SU_Normal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="0.00" numFmtId="165"/>
-    <numFmt formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;" numFmtId="166"/>
-    <numFmt formatCode="@" numFmtId="167"/>
+    <numFmt formatCode="@" numFmtId="166"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -230,11 +255,6 @@
       <family val="2"/>
       <sz val="10"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <sz val="10"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -253,16 +273,16 @@
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
-      <left style="medium">
+      <left style="thick">
         <color rgb="003C3C3C"/>
       </left>
-      <right style="medium">
+      <right style="thick">
         <color rgb="003C3C3C"/>
       </right>
-      <top style="medium">
+      <top style="thick">
         <color rgb="003C3C3C"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thick">
         <color rgb="003C3C3C"/>
       </bottom>
       <diagonal/>
@@ -293,17 +313,15 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="167" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="166" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -392,11 +410,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.2549019607843"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.76078431372549"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.96862745098039"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.22352941176471"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.22352941176471"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.3254901960784"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.7921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.0117647058824"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.25882352941177"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.25882352941177"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="1">
@@ -411,23 +429,24 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="b">
+      <c r="B2" s="1" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="4">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -439,7 +458,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="5">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -451,7 +470,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="6">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -463,7 +482,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="7">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -497,29 +516,29 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.63529411764706"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.9058823529412"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.2941176470588"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.22352941176471"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.22352941176471"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.67058823529412"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.0274509803922"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.3725490196078"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.25882352941177"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.25882352941177"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -527,18 +546,18 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="4">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -549,7 +568,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="5">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -560,7 +579,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="6">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -571,7 +590,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="7">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -582,18 +601,18 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="8">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="9">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -626,45 +645,45 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.85882352941177"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.81960784313726"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.3411764705882"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.5294117647059"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.1960784313725"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.7098039215686"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.9882352941176"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.0941176470588"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="14.1254901960784"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.34509803921569"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.20392156862745"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="14.6509803921569"/>
-    <col collapsed="false" hidden="false" max="257" min="13" style="1" width="9.22352941176471"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.22352941176471"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.89411764705882"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.85490196078431"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.4"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.5803921568627"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.2509803921569"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.7882352941176"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.043137254902"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.1450980392157"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="14.1843137254902"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.38039215686275"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.23921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="14.7137254901961"/>
+    <col collapsed="false" hidden="false" max="257" min="13" style="1" width="9.25882352941177"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.25882352941177"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="1">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>32</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -687,7 +706,7 @@
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -700,14 +719,14 @@
         <v>40</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
-      <c r="A3" s="6" t="s">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="3">
+      <c r="A3" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="5" t="s">
         <v>16</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -740,15 +759,15 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="E2" activeCellId="0" pane="topLeft" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.2156862745098"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="1" width="4.68235294117647"/>
-    <col collapsed="false" hidden="false" max="257" min="6" style="1" width="9.22352941176471"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.22352941176471"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.23921568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="1" width="4.70588235294118"/>
+    <col collapsed="false" hidden="false" max="257" min="6" style="1" width="9.25882352941177"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.25882352941177"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="1">
@@ -780,6 +799,77 @@
       </c>
       <c r="E2" s="1" t="n">
         <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C1" activeCellId="0" pane="topLeft" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.6078431372549"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="16.043137254902"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.2313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.18039215686274"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
+      <c r="A2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="3">
+      <c r="A3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>